<commit_message>
Fixed negative number conversion issue
</commit_message>
<xml_diff>
--- a/cpu_timing.xlsx
+++ b/cpu_timing.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\2021_Spring\ECEN5863\Homework\HW3_Practical\DE1-SoC_v.5.1.2_HWrevF_SystemCD\Demonstrations\SOC_FPGA\my_first_hps-fpga\hps-c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB35691-2568-401E-9A79-94291E36356A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D3E060-47C8-4EF6-B1B6-03F8B6F97B74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EEDD7A90-6C18-4CB0-A52A-F181465B4853}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEDD7A90-6C18-4CB0-A52A-F181465B4853}"/>
   </bookViews>
   <sheets>
     <sheet name="cpu_timing" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'cpu_timing'!$A$1:$E$61</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'cpu_timing'!$A$1:$F$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="13">
   <si>
     <t>Jan  1 00:01:20 de1soclinux my_first_hps: CPU_timing</t>
   </si>
@@ -65,11 +65,35 @@
   <si>
     <t>msec</t>
   </si>
+  <si>
+    <t>I2C Read Time</t>
+  </si>
+  <si>
+    <t>CPU Filter Proc Time</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>CPU Proc (artificial Load)</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>FPGA Handshaking</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,14 +123,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -126,14 +154,1175 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Jitter: CPU Filter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'cpu_timing'!$E$3:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>-9.9999999999999829E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.5999999999999991E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0000000000000052E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.099999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.1999999999999988E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.1999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0000000000000236E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0000000000000105E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0000000000000157E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.9999999999999724E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0000000000000236E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0000000000000079E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0000000000000079E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0000000000000052E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.0000000000000236E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-7.9999999999999776E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0000000000000157E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.9999999999999645E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.0000000000000184E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.0000000000000105E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.0000000000000131E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0000000000000052E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.000000000000021E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.0000000000000157E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.0000000000000131E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.8999999999999963E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0000000000000026E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.0000000000000131E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.0000000000000157E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0000000000000026E-5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.0000000000000052E-5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-4.9999999999999697E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.0000000000000079E-5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.0000000000000157E-5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.0000000000000131E-5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.000000000000021E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-3.9999999999999671E-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.0000000000000079E-5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.000000000000021E-5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.0000000000000052E-5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.0000000000000052E-5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.0000000000000105E-5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.0000000000000131E-5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.000000000000021E-5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.0000000000000157E-5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1.9999999999999619E-5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-2.0999999999999968E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-1.5999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-3.9999999999999671E-5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.0000000000000079E-5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-1.9999999999999619E-5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.0000000000000079E-5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.0000000000000236E-5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-1.9999999999999619E-5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.0000000000000079E-5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.0000000000000131E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-43E4-46DA-95C8-64855DA69CD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="739752424"/>
+        <c:axId val="739752752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="739752424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sample No.</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="739752752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="739752752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>msec</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="739752424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>116204</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>164782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C0C5C42-C2E6-4670-9B40-3E62624F8486}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{084F6BF8-149B-4904-82C9-7E536D76066E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="7">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="8">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Jan  1 00:01:20 de1soclinux my_first_hps: CPU_timing" tableColumnId="1"/>
       <queryTableField id="2" name="Total_Time" tableColumnId="2"/>
       <queryTableField id="3" name="I2C_Read_Time" tableColumnId="3"/>
       <queryTableField id="4" name="Filter_Time" tableColumnId="4"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="6"/>
       <queryTableField id="5" name="Units" tableColumnId="5"/>
     </queryTableFields>
   </queryTableRefresh>
@@ -141,14 +1330,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9AA8C4CF-1CF9-4A7B-8CC2-E36484ABAD59}" name="cpu_timing" displayName="cpu_timing" ref="A1:E61" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E61" xr:uid="{9D375EE0-7AC2-4971-9E04-75208E88B263}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5850BC5F-0703-4A54-A738-244B6AC86B66}" uniqueName="1" name="Jan  1 00:01:20 de1soclinux my_first_hps: CPU_timing" queryTableFieldId="1" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9AA8C4CF-1CF9-4A7B-8CC2-E36484ABAD59}" name="cpu_timing" displayName="cpu_timing" ref="A1:F61" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F61" xr:uid="{9D375EE0-7AC2-4971-9E04-75208E88B263}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{5850BC5F-0703-4A54-A738-244B6AC86B66}" uniqueName="1" name="Jan  1 00:01:20 de1soclinux my_first_hps: CPU_timing" queryTableFieldId="1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{EE484ADC-9DB5-45A6-B2BE-AB0A95D6FB31}" uniqueName="2" name="Total_Time" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{96CE6E3B-1EBA-4369-88DF-28382D5E3E7C}" uniqueName="3" name="I2C_Read_Time" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{C464F968-21A3-49DC-A161-50F72B07A550}" uniqueName="4" name="Filter_Time" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{93A94165-AFAB-4133-B405-7A3D3ACCCBEC}" uniqueName="5" name="Units" queryTableFieldId="5" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{DD0209CF-3903-4B64-843D-7B89327F4561}" uniqueName="6" name="Column1" queryTableFieldId="7" dataDxfId="0">
+      <calculatedColumnFormula>$D$40-cpu_timing[[#This Row],[Filter_Time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{93A94165-AFAB-4133-B405-7A3D3ACCCBEC}" uniqueName="5" name="Units" queryTableFieldId="5" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -451,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FCBB62-1B92-481C-95B0-8DF5453AD376}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H1" sqref="H1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,10 +1655,13 @@
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,10 +1675,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,11 +1700,22 @@
       <c r="D2">
         <v>1.737E-2</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-1.498E-2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(cpu_timing[I2C_Read_Time])</f>
+        <v>1.2375910000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,11 +1728,22 @@
       <c r="D3">
         <v>2.49E-3</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-9.9999999999999829E-5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <f>AVERAGE(D3:D61)</f>
+        <v>2.3993220338983049E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,11 +1756,21 @@
       <c r="D4">
         <v>2.8500000000000001E-3</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-4.5999999999999991E-4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2">
+        <v>6.0783050847457625E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,11 +1783,21 @@
       <c r="D5">
         <v>2.3700000000000001E-3</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>2.0000000000000052E-5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6.1498305084745769E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,11 +1810,15 @@
       <c r="D6">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-5.099999999999996E-4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,11 +1831,15 @@
       <c r="D7">
         <v>2.5100000000000001E-3</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-1.1999999999999988E-4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,11 +1852,15 @@
       <c r="D8">
         <v>2.7100000000000002E-3</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-3.1999999999999997E-4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,11 +1873,15 @@
       <c r="D9">
         <v>2.3E-3</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>9.0000000000000236E-5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,11 +1894,15 @@
       <c r="D10">
         <v>2.3500000000000001E-3</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>4.0000000000000105E-5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,11 +1915,15 @@
       <c r="D11">
         <v>2.33E-3</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>6.0000000000000157E-5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,11 +1936,15 @@
       <c r="D12">
         <v>2.4499999999999999E-3</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-5.9999999999999724E-5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,11 +1957,15 @@
       <c r="D13">
         <v>2.3E-3</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>9.0000000000000236E-5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,11 +1978,15 @@
       <c r="D14">
         <v>2.3600000000000001E-3</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>3.0000000000000079E-5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,11 +1999,15 @@
       <c r="D15">
         <v>2.3600000000000001E-3</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>3.0000000000000079E-5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,11 +2020,15 @@
       <c r="D16">
         <v>2.3700000000000001E-3</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>2.0000000000000052E-5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,11 +2041,15 @@
       <c r="D17">
         <v>2.3E-3</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>9.0000000000000236E-5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,11 +2062,15 @@
       <c r="D18">
         <v>2.47E-3</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-7.9999999999999776E-5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,11 +2083,15 @@
       <c r="D19">
         <v>2.33E-3</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>6.0000000000000157E-5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,11 +2104,15 @@
       <c r="D20">
         <v>2.4199999999999998E-3</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-2.9999999999999645E-5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,11 +2125,15 @@
       <c r="D21">
         <v>2.32E-3</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>7.0000000000000184E-5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,11 +2146,15 @@
       <c r="D22">
         <v>2.3500000000000001E-3</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>4.0000000000000105E-5</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,11 +2167,15 @@
       <c r="D23">
         <v>2.3400000000000001E-3</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>5.0000000000000131E-5</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,11 +2188,15 @@
       <c r="D24">
         <v>2.3700000000000001E-3</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>2.0000000000000052E-5</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,11 +2209,15 @@
       <c r="D25">
         <v>2.31E-3</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>8.000000000000021E-5</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,11 +2230,15 @@
       <c r="D26">
         <v>2.33E-3</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>6.0000000000000157E-5</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,11 +2251,15 @@
       <c r="D27">
         <v>2.3400000000000001E-3</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>5.0000000000000131E-5</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -938,11 +2272,15 @@
       <c r="D28">
         <v>2.5799999999999998E-3</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-1.8999999999999963E-4</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,11 +2293,15 @@
       <c r="D29">
         <v>2.3800000000000002E-3</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>1.0000000000000026E-5</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,11 +2314,15 @@
       <c r="D30">
         <v>2.3400000000000001E-3</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>5.0000000000000131E-5</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,11 +2335,15 @@
       <c r="D31">
         <v>2.33E-3</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>6.0000000000000157E-5</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,11 +2356,15 @@
       <c r="D32">
         <v>2.3900000000000002E-3</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,11 +2377,15 @@
       <c r="D33">
         <v>2.3800000000000002E-3</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>1.0000000000000026E-5</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,11 +2398,15 @@
       <c r="D34">
         <v>2.3700000000000001E-3</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>2.0000000000000052E-5</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -1057,11 +2419,15 @@
       <c r="D35">
         <v>2.3900000000000002E-3</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1074,11 +2440,15 @@
       <c r="D36">
         <v>2.4399999999999999E-3</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-4.9999999999999697E-5</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -1091,11 +2461,15 @@
       <c r="D37">
         <v>2.3600000000000001E-3</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>3.0000000000000079E-5</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,11 +2482,15 @@
       <c r="D38">
         <v>2.33E-3</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>6.0000000000000157E-5</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,11 +2503,15 @@
       <c r="D39">
         <v>2.3400000000000001E-3</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>5.0000000000000131E-5</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -1142,11 +2524,15 @@
       <c r="D40">
         <v>2.3900000000000002E-3</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -1159,11 +2545,15 @@
       <c r="D41">
         <v>2.31E-3</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>8.000000000000021E-5</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -1176,11 +2566,15 @@
       <c r="D42">
         <v>2.4299999999999999E-3</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-3.9999999999999671E-5</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -1193,11 +2587,15 @@
       <c r="D43">
         <v>2.3600000000000001E-3</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>3.0000000000000079E-5</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -1210,11 +2608,15 @@
       <c r="D44">
         <v>2.31E-3</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>8.000000000000021E-5</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1227,11 +2629,15 @@
       <c r="D45">
         <v>2.3700000000000001E-3</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>2.0000000000000052E-5</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -1244,11 +2650,15 @@
       <c r="D46">
         <v>2.3700000000000001E-3</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>2.0000000000000052E-5</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1261,11 +2671,15 @@
       <c r="D47">
         <v>2.3500000000000001E-3</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>4.0000000000000105E-5</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -1278,11 +2692,15 @@
       <c r="D48">
         <v>2.3400000000000001E-3</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>5.0000000000000131E-5</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -1295,11 +2713,15 @@
       <c r="D49">
         <v>2.31E-3</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>8.000000000000021E-5</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -1312,11 +2734,15 @@
       <c r="D50">
         <v>2.33E-3</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>6.0000000000000157E-5</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -1329,11 +2755,15 @@
       <c r="D51">
         <v>2.4099999999999998E-3</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-1.9999999999999619E-5</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -1346,11 +2776,15 @@
       <c r="D52">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-2.0999999999999968E-4</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -1363,11 +2797,15 @@
       <c r="D53">
         <v>2.5500000000000002E-3</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-1.5999999999999999E-4</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,11 +2818,15 @@
       <c r="D54">
         <v>2.4299999999999999E-3</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-3.9999999999999671E-5</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -1397,11 +2839,15 @@
       <c r="D55">
         <v>2.3600000000000001E-3</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>3.0000000000000079E-5</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -1414,11 +2860,15 @@
       <c r="D56">
         <v>2.4099999999999998E-3</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-1.9999999999999619E-5</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,11 +2881,15 @@
       <c r="D57">
         <v>2.3600000000000001E-3</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>3.0000000000000079E-5</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,11 +2902,15 @@
       <c r="D58">
         <v>2.3E-3</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>9.0000000000000236E-5</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -1465,11 +2923,15 @@
       <c r="D59">
         <v>2.4099999999999998E-3</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>-1.9999999999999619E-5</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -1482,11 +2944,15 @@
       <c r="D60">
         <v>2.3600000000000001E-3</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>3.0000000000000079E-5</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -1499,14 +2965,19 @@
       <c r="D61">
         <v>2.3400000000000001E-3</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61">
+        <f>$D$40-cpu_timing[[#This Row],[Filter_Time]]</f>
+        <v>5.0000000000000131E-5</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>